<commit_message>
Fix rs1_enable of is_lui to 1 in `Decode.xlsx`
</commit_message>
<xml_diff>
--- a/docs/Decode.xlsx
+++ b/docs/Decode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TH\project\cod19grp73\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA424DA-C139-479A-AD48-CAB0CB35977F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838C9604-93DF-48A6-86C7-6B3A35AD1CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{FBB57B1D-E129-4906-A75B-2C3DC31596A6}"/>
   </bookViews>
@@ -834,7 +834,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C92" sqref="C92"/>
+      <selection pane="topRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -889,7 +889,7 @@
         <v>52</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>

</xml_diff>